<commit_message>
Bandwidth after RCM ordering
</commit_message>
<xml_diff>
--- a/CombBLAS/Ordering/RCM-exp.xlsx
+++ b/CombBLAS/Ordering/RCM-exp.xlsx
@@ -4,10 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14460" tabRatio="500"/>
+    <workbookView xWindow="980" yWindow="540" windowWidth="25600" windowHeight="14460" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="new run" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="8">
   <si>
     <t>delaunay_n24.mtx</t>
   </si>
@@ -91,24 +94,39 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -440,8 +458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -626,17 +644,17 @@
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="G11" s="1" t="s">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="G11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -651,4 +669,438 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="3" width="14.5" customWidth="1"/>
+    <col min="4" max="6" width="14.1640625" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="2"/>
+      <c r="K1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>3.83</v>
+      </c>
+      <c r="D2">
+        <v>0.74</v>
+      </c>
+      <c r="G2">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="J2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2">
+        <v>3.83</v>
+      </c>
+      <c r="L2">
+        <v>0.74</v>
+      </c>
+      <c r="M2">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>3661</v>
+      </c>
+      <c r="D3">
+        <v>84</v>
+      </c>
+      <c r="G3">
+        <v>1720</v>
+      </c>
+      <c r="J3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3">
+        <v>3661</v>
+      </c>
+      <c r="L3">
+        <v>84</v>
+      </c>
+      <c r="M3">
+        <v>1720</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>27.844999999999999</v>
+      </c>
+      <c r="E6">
+        <v>9.0641400000000001</v>
+      </c>
+      <c r="F6">
+        <v>0.69417899999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>4.8609200000000001</v>
+      </c>
+      <c r="E7">
+        <v>2.36754</v>
+      </c>
+      <c r="F7">
+        <v>0.258353</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8">
+        <v>16</v>
+      </c>
+      <c r="D8">
+        <v>2.27935</v>
+      </c>
+      <c r="E8">
+        <v>0.74688500000000002</v>
+      </c>
+      <c r="F8">
+        <v>0.13431299999999999</v>
+      </c>
+      <c r="J8">
+        <v>24</v>
+      </c>
+      <c r="L8">
+        <v>2.3612799999999998</v>
+      </c>
+      <c r="M8">
+        <v>80.499399999999994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9">
+        <v>64</v>
+      </c>
+      <c r="D9">
+        <v>0.90815999999999997</v>
+      </c>
+      <c r="E9">
+        <v>0.25439000000000001</v>
+      </c>
+      <c r="F9">
+        <v>0.74748800000000004</v>
+      </c>
+      <c r="J9">
+        <v>96</v>
+      </c>
+      <c r="L9">
+        <v>0.85255400000000003</v>
+      </c>
+      <c r="M9">
+        <v>25.313199999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10">
+        <v>256</v>
+      </c>
+      <c r="D10">
+        <v>0.41655799999999998</v>
+      </c>
+      <c r="E10">
+        <v>0.10340000000000001</v>
+      </c>
+      <c r="F10">
+        <v>9.3743800000000004</v>
+      </c>
+      <c r="J10">
+        <v>384</v>
+      </c>
+      <c r="L10">
+        <v>0.34128399999999998</v>
+      </c>
+      <c r="M10">
+        <v>13.709099999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11">
+        <v>1024</v>
+      </c>
+      <c r="D11">
+        <v>0.46089200000000002</v>
+      </c>
+      <c r="J11">
+        <v>1536</v>
+      </c>
+      <c r="L11">
+        <v>0.14841799999999999</v>
+      </c>
+      <c r="M11">
+        <v>6.2482800000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="B13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="J13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="J13:M13"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="3" width="14.5" customWidth="1"/>
+    <col min="4" max="6" width="14.1640625" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10">
+        <v>256</v>
+      </c>
+      <c r="D10">
+        <v>0.51919800000000005</v>
+      </c>
+      <c r="E10">
+        <v>0.172929</v>
+      </c>
+      <c r="F10">
+        <v>0.17516000000000001</v>
+      </c>
+      <c r="G10">
+        <v>25.7102</v>
+      </c>
+      <c r="H10">
+        <v>6.48163</v>
+      </c>
+      <c r="I10">
+        <v>4.2730800000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11">
+        <v>1024</v>
+      </c>
+      <c r="D11">
+        <v>0.349325</v>
+      </c>
+      <c r="E11">
+        <v>5.7992500000000002E-2</v>
+      </c>
+      <c r="F11">
+        <v>1.3085500000000001</v>
+      </c>
+      <c r="G11">
+        <v>11.2601</v>
+      </c>
+      <c r="H11">
+        <v>3.4065099999999999</v>
+      </c>
+      <c r="I11">
+        <v>58.635399999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="B13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="J13:M13"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E3:H5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="3" spans="5:8">
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>90</v>
+      </c>
+      <c r="H3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="5:8">
+      <c r="E4">
+        <v>16</v>
+      </c>
+      <c r="F4">
+        <v>17.945</v>
+      </c>
+      <c r="H4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="5:8">
+      <c r="E5">
+        <v>256</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>